<commit_message>
added the gall_interaction_network file
</commit_message>
<xml_diff>
--- a/Gall_Interaction_network.xlsx
+++ b/Gall_Interaction_network.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="800" windowWidth="20860" windowHeight="14580" tabRatio="740" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="15320" tabRatio="740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Interaction_Matrix" sheetId="7" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="PG unknown" sheetId="8" r:id="rId8"/>
     <sheet name="SG 2 unknown Cecidomyiidae" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="130407"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,135 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="130">
+  <si>
+    <t>#Currently unknown whether this gall has been described or not</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>aSG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>aSG, apical shoot gall</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>aSG larva</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hymenoptera</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Platygastroidea</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Platygasteridae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Platygaster</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Platygaster sp. 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Torymus sp. connection from 2011 gall collections</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ichneumonid sp.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No data for yet</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Torymus sp. male</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Torymus sp. female</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>from 2011 gall collections</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>from 2011 gall collections</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Torymidae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Torymus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iteomyia larva</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hymenoptera</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pteromalidae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mesopolobus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mesopolobus sp.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hymenoptera</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chalcidoidea</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Platygastroidea</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Platygastridae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Platygaster</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>californica?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>egg parasitoid</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hymenoptera</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>#Currently unknown whether this gall has been described or not. Sometimes difficult to distinguish from aSG when dried and collected</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -201,19 +329,27 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>#Currently unknown whether this gall has been described or not</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>aSG</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>aSG, apical shoot gall</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>aSG larva</t>
+    <t>Pteromalidae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Moth inquiline</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lepidoptera</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mesopolobus? Or Gastrancistrus?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pontania californica adult</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -221,19 +357,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Platygastroidea</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Platygasteridae</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Platygaster</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Platygaster sp. 2</t>
+    <t>yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>noticeable darkened club at end of antenna and yellow band on abdomen; former morphospecies Chal_MetGrn_YB</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -418,90 +546,6 @@
   </si>
   <si>
     <t>vLG</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Iteomyia larva</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hymenoptera</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pteromalidae</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mesopolobus</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mesopolobus sp.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hymenoptera</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chalcidoidea</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Platygastroidea</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Platygastridae</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Platygaster</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>californica?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>egg parasitoid</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hymenoptera</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pteromalidae</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Moth inquiline</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lepidoptera</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mesopolobus? Or Gastrancistrus?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pontania californica adult</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hymenoptera</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yes</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -543,12 +587,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,50 +923,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="2.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="91">
+    <row r="1" spans="1:11" ht="92">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>102</v>
+        <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>89</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -939,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -947,10 +998,16 @@
       <c r="I2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -976,10 +1033,13 @@
       <c r="I3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -994,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1005,29 +1065,37 @@
       <c r="I4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>55</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>56</v>
+      </c>
+      <c r="K8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1041,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="DV1" workbookViewId="0">
+      <selection activeCell="DZ6" sqref="DZ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1055,42 +1123,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="I2" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="J2" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1098,25 +1166,25 @@
         <v>378</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="G3" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="H3" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="I3" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1124,22 +1192,25 @@
         <v>401</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="E4" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>101</v>
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1147,31 +1218,31 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>106</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>107</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>109</v>
+        <v>30</v>
       </c>
       <c r="K5" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1179,22 +1250,22 @@
         <v>408</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="E6" t="s">
-        <v>110</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="H6" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1202,13 +1273,13 @@
         <v>405</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1216,19 +1287,19 @@
         <v>381</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1236,19 +1307,19 @@
         <v>411</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1256,23 +1327,68 @@
         <v>410</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>5</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>380</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>402</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1300,42 +1416,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="I2" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="J2" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1343,22 +1459,22 @@
         <v>376</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="G3" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="I3" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1366,19 +1482,19 @@
         <v>380</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="H4" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1386,22 +1502,22 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1409,23 +1525,22 @@
         <v>415</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="H6" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="I6" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1453,42 +1568,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="I2" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="J2" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1496,19 +1611,19 @@
         <v>277</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1516,22 +1631,22 @@
         <v>377</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1539,19 +1654,19 @@
         <v>409</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1559,22 +1674,22 @@
         <v>403</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="G6" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1582,17 +1697,16 @@
         <v>414</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1620,42 +1734,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="I2" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="J2" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1663,26 +1777,25 @@
         <v>404</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1698,7 +1811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1706,42 +1819,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="I2" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="J2" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1749,14 +1862,13 @@
         <v>412</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1780,42 +1892,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="I2" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="J2" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1823,26 +1935,25 @@
         <v>402</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1864,7 +1975,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1891,42 +2001,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="I2" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="J2" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1934,11 +2044,10 @@
         <v>413</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
added info to genotype networks
</commit_message>
<xml_diff>
--- a/Gall_Interaction_network.xlsx
+++ b/Gall_Interaction_network.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="15320" tabRatio="740" activeTab="1"/>
+    <workbookView xWindow="8120" yWindow="-80" windowWidth="21600" windowHeight="15320" tabRatio="740" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Interaction_Matrix" sheetId="7" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="PG unknown" sheetId="8" r:id="rId8"/>
     <sheet name="SG 2 unknown Cecidomyiidae" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="130407"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,155 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="137">
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lepidoptera</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lestodiplosis?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diptera</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cecidomyiidae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#Currently unknown whether this gall has been described or not.  The larva look superficially identifical to Rabdophaga salicisbattatus larva (long spatula), and they may be the same (but I'm keeping them separate for now).</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SG 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>currently unknown whether this is the female of the species attacking the rosette galls (Rabdophaga salicisbattatus)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mymaridae sp. 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hymenoptera</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chalcidoidea</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mymaridae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iteomyia salicisverruca</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rabdophaga salicisbrassicoides</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pontania californica</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>other orange larva</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Torymus sp. 2 female</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hymenoptera</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#Gall species identification from Russo's "Field guide to plants galls of California and other Western states"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Picture Organized</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rabdophaga rosette</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rabdophaga</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>salicisbrassicoides</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Picture organized</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Torymus male</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hymenoptera</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Torymidae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Torymus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#Gall species identification based on Russo's "Field guide to plant galls of California and other western states"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eurytoma female</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hymenoptera</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chalcidoidea</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eurytomidae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>#Currently unknown whether this gall has been described or not</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -185,39 +333,211 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>Eurytoma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>yes</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>Eulophidae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eulophid female</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Species_Code</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nickname</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Superfamily</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Family</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Genus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Species</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#Gall species identification from Haggard &amp; Haggard's "Insects of the Pacific Northwest" and Gagne's "Plant feeding gall midges of North America"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biology</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Order</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diptera</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cecidomyiidae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iteomyia</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>salicisverruca</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other names</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>vLG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lathrostizus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hymenoptera</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ichneumoidea</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ichneumonidae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lathrostizus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rabdophaga salicisbattatus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>twG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Platygaster sp.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mymaridae sp.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eulophid sp.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Moth inquiline</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Torymus sp.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eurytoma sp.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tenthredinidae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Pontania </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>californica</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pontania californica prepupa</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pontania californica larva</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>typically all shrivelled up</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pteromalid sp. 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rabdophaga larva</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cecidomyiidae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rabdophaga</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>salicisbrassicoides</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pteromalidae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Moth inquiline</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Lepidoptera</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Lestodiplosis?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Diptera</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cecidomyiidae</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>#Currently unknown whether this gall has been described or not.  The larva look superficially identifical to Rabdophaga salicisbattatus larva (long spatula), and they may be the same (but I'm keeping them separate for now).</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SG 2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>currently unknown whether this is the female of the species attacking the rosette galls (Rabdophaga salicisbattatus)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mymaridae sp. 1</t>
+    <t>Mesopolobus? Or Gastrancistrus?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pontania californica adult</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -225,142 +545,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Chalcidoidea</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mymaridae</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Iteomyia salicisverruca</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rabdophaga salicisbrassicoides</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pontania californica</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rabdophaga salicisbattatus</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>twG</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PG</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Platygaster sp.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mymaridae sp.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eulophid sp.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Moth inquiline</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Torymus sp.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eurytoma sp.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tenthredinidae</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Pontania </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>californica</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pontania californica prepupa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pontania californica larva</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>typically all shrivelled up</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pteromalid sp. 2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rabdophaga larva</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SG</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cecidomyiidae</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rabdophaga</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>salicisbrassicoides</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pteromalidae</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Moth inquiline</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lepidoptera</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mesopolobus? Or Gastrancistrus?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>yes</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Pontania californica adult</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hymenoptera</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>noticeable darkened club at end of antenna and yellow band on abdomen; former morphospecies Chal_MetGrn_YB</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -386,166 +574,6 @@
   </si>
   <si>
     <t>Lestodiplosis sp.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Torymus sp. 2 female</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hymenoptera</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>#Gall species identification from Russo's "Field guide to plants galls of California and other Western states"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Picture Organized</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>rG</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rabdophaga rosette</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rabdophaga</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>salicisbrassicoides</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Picture organized</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Torymus male</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hymenoptera</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Torymidae</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Torymus</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NEED</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>#Gall species identification based on Russo's "Field guide to plant galls of California and other western states"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eurytoma female</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hymenoptera</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chalcidoidea</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eurytomidae</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eurytoma</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>yes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eulophidae</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Eulophid female</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Species_Code</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nickname</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Superfamily</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Family</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Genus</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Species</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Notes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>#Gall species identification from Haggard &amp; Haggard's "Insects of the Pacific Northwest" and Gagne's "Plant feeding gall midges of North America"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biology</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Order</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Diptera</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cecidomyiidae</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Iteomyia</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>salicisverruca</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Other names</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>vLG</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -937,42 +965,42 @@
   <sheetData>
     <row r="1" spans="1:11" ht="92">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1002,12 +1030,12 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1039,7 +1067,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1071,17 +1099,17 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1089,13 +1117,14 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="K8" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1111,7 +1140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="DV1" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="DZ6" sqref="DZ6"/>
     </sheetView>
   </sheetViews>
@@ -1123,42 +1152,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="K2" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1166,25 +1195,25 @@
         <v>378</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="H3" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="I3" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1192,25 +1221,25 @@
         <v>401</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="K4" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1218,31 +1247,31 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="K5" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1250,22 +1279,22 @@
         <v>408</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1273,13 +1302,13 @@
         <v>405</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1287,19 +1316,19 @@
         <v>381</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1307,19 +1336,19 @@
         <v>411</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1327,19 +1356,19 @@
         <v>410</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G10" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1347,22 +1376,22 @@
         <v>380</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="K11" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1370,25 +1399,26 @@
         <v>402</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="H12" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="K12" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1402,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1416,42 +1446,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="K2" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1459,22 +1489,22 @@
         <v>376</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="H3" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1482,19 +1512,19 @@
         <v>380</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1502,22 +1532,22 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="K5" t="s">
-        <v>84</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1525,22 +1555,34 @@
         <v>415</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="I6" t="s">
-        <v>88</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1554,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1568,42 +1610,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="K2" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1611,19 +1653,19 @@
         <v>277</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1631,22 +1673,22 @@
         <v>377</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="I4" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="K4" t="s">
-        <v>68</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1654,19 +1696,19 @@
         <v>409</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1674,22 +1716,22 @@
         <v>403</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1697,16 +1739,37 @@
         <v>414</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>416</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1734,42 +1797,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="K2" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1777,25 +1840,26 @@
         <v>404</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="E3" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="I3" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1819,42 +1883,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="K2" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1862,13 +1926,14 @@
         <v>412</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1892,42 +1957,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="K2" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1935,25 +2000,26 @@
         <v>402</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1975,6 +2041,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2001,42 +2068,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="K2" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2044,10 +2111,11 @@
         <v>413</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>